<commit_message>
add constraints and objective
</commit_message>
<xml_diff>
--- a/code/ANRs.xlsx
+++ b/code/ANRs.xlsx
@@ -1,21 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/Library/CloudStorage/OneDrive-IdahoNationalLaboratory/Documents/Research/Hydrogen from Nuclear/code/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1DBE88-2681-B844-B8E1-8ADECFEBAC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="2920" yWindow="500" windowWidth="30060" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="FOAK"/>
-    <sheet r:id="rId2" sheetId="2" name="NOAK"/>
+    <sheet name="FOAK" sheetId="1" r:id="rId1"/>
+    <sheet name="NOAK" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>Reactor</t>
   </si>
@@ -90,13 +109,15 @@
   </si>
   <si>
     <t>Learning rate</t>
+  </si>
+  <si>
+    <t>Life (y)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,71 +172,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -226,10 +240,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -267,71 +281,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -359,7 +373,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -382,11 +396,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -395,13 +409,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -411,7 +425,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -420,7 +434,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -429,7 +443,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -437,10 +451,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -505,371 +519,387 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="13" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="18" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="23.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="18" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="18" width="30.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="16" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="16" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="16" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="16" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="18" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="18" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="18" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="16" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.83203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.1640625" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+      <c r="R1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>77</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>250</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>15.4</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>0.31</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>20</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>0.4</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <v>24</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="10">
         <v>302</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="10">
         <v>5535000</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="10">
         <v>115000</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="10">
         <v>12</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="8">
         <v>0.75</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="7">
         <v>9</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="Q2" s="7">
         <v>38500</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="R2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>164</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>350</v>
       </c>
-      <c r="E3" s="9">
-        <v>32.8</v>
-      </c>
-      <c r="F3" s="10">
+      <c r="E3" s="8">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="F3" s="9">
         <v>0.47</v>
       </c>
-      <c r="G3" s="9">
-        <v>0.897</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="G3" s="8">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H3" s="10">
         <v>20</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>6</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <v>984</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>950</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>7500000</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="10">
         <v>164000</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="10">
         <v>4</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="7">
         <v>0</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="7">
         <v>13</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="7">
         <v>82000</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+      <c r="R3" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>80</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>200</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>32</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>4</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0.751</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>20</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <v>2.4</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <v>48</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="10">
         <v>750</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <v>4569000</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="10">
         <v>100000</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="10">
         <v>12</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <v>0</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="7">
         <v>13</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="Q4" s="7">
         <v>40000</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+      <c r="R4" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>141</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>300</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>28.2</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>0.47</v>
       </c>
-      <c r="G5" s="9">
-        <v>0.936</v>
-      </c>
-      <c r="H5" s="11">
+      <c r="G5" s="8">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H5" s="10">
         <v>20</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>0.6</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>84.6</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
         <v>700</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <v>4091000</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="10">
         <v>85000</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="10">
         <v>12</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="8">
         <v>0.5</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="7">
         <v>11</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="7">
         <v>70500</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
+      <c r="R5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>6.7</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>20</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>2.7</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>0.33</v>
       </c>
-      <c r="G6" s="9">
-        <v>0.897</v>
-      </c>
-      <c r="H6" s="11">
+      <c r="G6" s="8">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H6" s="10">
         <v>20</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>6</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <v>24</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <v>630</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <v>10902000</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="10">
         <v>264000</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="10">
         <v>12</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>0</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="7">
         <v>0</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="Q6" s="7">
         <v>3350</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="12"/>
+      <c r="R6" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -877,413 +907,435 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="13" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="15" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="16" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="16" width="30.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="16" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="16" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="16" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="16" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="16" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="16" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="16" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.1640625" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+      <c r="R1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>77</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>250</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>15.4</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>0.31</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>20</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>0.4</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <v>24</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="10">
         <v>302</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="10">
         <f>FOAK!L2*(1-NOAK!$B$9)</f>
-      </c>
-      <c r="M2" s="11">
+        <v>4937220</v>
+      </c>
+      <c r="M2" s="10">
         <v>115000</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="10">
         <v>12</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="8">
         <v>0.75</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="7">
         <v>9</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="Q2" s="7">
         <v>38500</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="R2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>164</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>350</v>
       </c>
-      <c r="E3" s="9">
-        <v>32.8</v>
-      </c>
-      <c r="F3" s="10">
+      <c r="E3" s="8">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="F3" s="9">
         <v>0.47</v>
       </c>
-      <c r="G3" s="9">
-        <v>0.897</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="G3" s="8">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H3" s="10">
         <v>20</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="7">
         <v>6</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="7">
         <v>984</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>950</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <f>FOAK!L3*(1-NOAK!$B$9)</f>
-      </c>
-      <c r="M3" s="11">
+        <v>6690000</v>
+      </c>
+      <c r="M3" s="10">
         <v>164000</v>
       </c>
-      <c r="N3" s="11">
+      <c r="N3" s="10">
         <v>4</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="7">
         <v>0</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="7">
         <v>13</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="7">
         <v>82000</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
+      <c r="R3" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>80</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>200</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>32</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>4</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0.751</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>20</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <v>2.4</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <v>48</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="10">
         <v>750</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <f>FOAK!L4*(1-NOAK!$B$9)</f>
-      </c>
-      <c r="M4" s="11">
+        <v>4075548</v>
+      </c>
+      <c r="M4" s="10">
         <v>100000</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="10">
         <v>12</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="7">
         <v>0</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="7">
         <v>13</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="Q4" s="7">
         <v>40000</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
+      <c r="R4" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>141</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>300</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>28.2</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>0.47</v>
       </c>
-      <c r="G5" s="9">
-        <v>0.936</v>
-      </c>
-      <c r="H5" s="11">
+      <c r="G5" s="8">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H5" s="10">
         <v>20</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>0.6</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>84.6</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
         <v>700</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L5" s="10">
         <f>FOAK!L5*(1-NOAK!$B$9)</f>
-      </c>
-      <c r="M5" s="11">
+        <v>3649172</v>
+      </c>
+      <c r="M5" s="10">
         <v>85000</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="10">
         <v>12</v>
       </c>
-      <c r="O5" s="9">
+      <c r="O5" s="8">
         <v>0.5</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="7">
         <v>11</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="7">
         <v>70500</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
+      <c r="R5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>6.7</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>20</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>2.7</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>0.33</v>
       </c>
-      <c r="G6" s="9">
-        <v>0.897</v>
-      </c>
-      <c r="H6" s="11">
+      <c r="G6" s="8">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H6" s="10">
         <v>20</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>6</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <v>24</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <v>630</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="10">
         <f>FOAK!L6*(1-NOAK!$B$9)</f>
-      </c>
-      <c r="M6" s="11">
+        <v>9724584</v>
+      </c>
+      <c r="M6" s="10">
         <v>264000</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="10">
         <v>12</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="7">
         <v>0</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="7">
         <v>0</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="Q6" s="7">
         <v>3350</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1" t="s">
+      <c r="R6" s="7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+    </row>
+    <row r="8" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+    </row>
+    <row r="9" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>0.108</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Wrong calculation of total elec capacity for HTSE modules, needed to include ANR Thermal efficiency, careful with other types of h2 modules diff calc., corrected thermal eff htgr pbr in anr sheet
</commit_message>
<xml_diff>
--- a/code/ANRs.xlsx
+++ b/code/ANRs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/Library/CloudStorage/OneDrive-IdahoNationalLaboratory/Documents/Research/Hydrogen from Nuclear/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57522F6-6510-7347-B40B-EE60C73129F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F05A2BC-7D24-8940-A737-6B5A14169B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="500" windowWidth="30060" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31340" yWindow="1460" windowWidth="30060" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOAK" sheetId="1" r:id="rId1"/>
@@ -525,8 +525,8 @@
   </sheetPr>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -722,8 +722,8 @@
       <c r="E4" s="7">
         <v>32</v>
       </c>
-      <c r="F4" s="10">
-        <v>4</v>
+      <c r="F4" s="9">
+        <v>0.4</v>
       </c>
       <c r="G4" s="8">
         <v>0.751</v>

</xml_diff>

<commit_message>
update VOM, now include fuel costs
</commit_message>
<xml_diff>
--- a/code/ANRs.xlsx
+++ b/code/ANRs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FB6F26-9605-43C8-8B61-DBB53B3C9F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465FE2E8-85F1-4DBC-A628-6F22AC94F436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOAK" sheetId="1" r:id="rId1"/>
@@ -547,8 +547,8 @@
   </sheetPr>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -666,7 +666,8 @@
         <v>12</v>
       </c>
       <c r="O2" s="8">
-        <v>0.75</v>
+        <f>0.75+9</f>
+        <v>9.75</v>
       </c>
       <c r="P2" s="7">
         <v>38500</v>
@@ -719,7 +720,7 @@
         <v>4</v>
       </c>
       <c r="O3" s="7">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="P3" s="7">
         <v>82000</v>
@@ -772,7 +773,7 @@
         <v>12</v>
       </c>
       <c r="O4" s="7">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="P4" s="7">
         <v>40000</v>
@@ -825,7 +826,7 @@
         <v>12</v>
       </c>
       <c r="O5" s="8">
-        <v>0.5</v>
+        <v>11.5</v>
       </c>
       <c r="P5" s="7">
         <v>70500</v>
@@ -1484,7 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1361B2-645F-498E-85AE-774371151F01}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
NOAK data in spreadsheet, post-process noak results
</commit_message>
<xml_diff>
--- a/code/ANRs.xlsx
+++ b/code/ANRs.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C51FC24-861B-4240-BF01-22E250745B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89668816-D859-4561-9A74-9A463BB01239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FOAK" sheetId="1" r:id="rId1"/>
+    <sheet name="NOAK" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>Reactor</t>
   </si>
@@ -105,6 +106,15 @@
   </si>
   <si>
     <t>Life (y)</t>
+  </si>
+  <si>
+    <t>CAPEX $/MWe_foak</t>
+  </si>
+  <si>
+    <t>FOPEX $/MWe-y_foak</t>
+  </si>
+  <si>
+    <t>VOM in $/MWh-e_foak</t>
   </si>
 </sst>
 </file>
@@ -159,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -187,7 +197,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -501,8 +510,8 @@
   </sheetPr>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -526,34 +535,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -568,21 +577,21 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="5">
@@ -628,15 +637,15 @@
       <c r="P2" s="5">
         <v>38500</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="Q2">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="5">
@@ -686,10 +695,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="11" t="s">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="5">
@@ -739,10 +748,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="5">
@@ -787,15 +796,15 @@
       <c r="P5" s="5">
         <v>70500</v>
       </c>
-      <c r="Q5" s="11">
+      <c r="Q5">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="11" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="4">
@@ -845,23 +854,428 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
       <c r="P7" s="6"/>
-      <c r="Q7" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{788C6308-E7B4-4A56-9A52-B737D158C32F}">
+  <dimension ref="A1:T6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="12" max="12" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5">
+        <v>77</v>
+      </c>
+      <c r="D2" s="5">
+        <v>250</v>
+      </c>
+      <c r="E2" s="4">
+        <v>15.4</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>20</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="J2" s="5">
+        <v>24</v>
+      </c>
+      <c r="K2" s="5">
+        <v>302</v>
+      </c>
+      <c r="L2" s="5">
+        <v>5535000</v>
+      </c>
+      <c r="M2" s="5">
+        <v>115000</v>
+      </c>
+      <c r="N2" s="5">
+        <v>12</v>
+      </c>
+      <c r="O2" s="4">
+        <f>0.75+9</f>
+        <v>9.75</v>
+      </c>
+      <c r="P2" s="4">
+        <f>L2*0.8</f>
+        <v>4428000</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>M2*0.8</f>
+        <v>92000</v>
+      </c>
+      <c r="R2" s="4">
+        <f>O2*0.8</f>
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="S2" s="5">
+        <v>38500</v>
+      </c>
+      <c r="T2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5">
+        <v>164</v>
+      </c>
+      <c r="D3" s="5">
+        <v>350</v>
+      </c>
+      <c r="E3" s="4">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H3" s="5">
+        <v>20</v>
+      </c>
+      <c r="I3" s="5">
+        <v>6</v>
+      </c>
+      <c r="J3" s="5">
+        <v>984</v>
+      </c>
+      <c r="K3" s="5">
+        <v>950</v>
+      </c>
+      <c r="L3" s="5">
+        <v>7500000</v>
+      </c>
+      <c r="M3" s="5">
+        <v>164000</v>
+      </c>
+      <c r="N3" s="5">
+        <v>4</v>
+      </c>
+      <c r="O3" s="5">
+        <v>13</v>
+      </c>
+      <c r="P3" s="4">
+        <f t="shared" ref="P3:P6" si="0">L3*0.8</f>
+        <v>6000000</v>
+      </c>
+      <c r="Q3" s="4">
+        <f t="shared" ref="Q3:Q6" si="1">M3*0.8</f>
+        <v>131200</v>
+      </c>
+      <c r="R3" s="4">
+        <f t="shared" ref="R3:R6" si="2">O3*0.8</f>
+        <v>10.4</v>
+      </c>
+      <c r="S3" s="5">
+        <v>82000</v>
+      </c>
+      <c r="T3" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5">
+        <v>80</v>
+      </c>
+      <c r="D4" s="5">
+        <v>200</v>
+      </c>
+      <c r="E4" s="5">
+        <v>32</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0.751</v>
+      </c>
+      <c r="H4" s="5">
+        <v>20</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="J4" s="5">
+        <v>48</v>
+      </c>
+      <c r="K4" s="5">
+        <v>750</v>
+      </c>
+      <c r="L4" s="5">
+        <v>4569000</v>
+      </c>
+      <c r="M4" s="5">
+        <v>100000</v>
+      </c>
+      <c r="N4" s="5">
+        <v>12</v>
+      </c>
+      <c r="O4" s="5">
+        <v>13</v>
+      </c>
+      <c r="P4" s="4">
+        <f t="shared" si="0"/>
+        <v>3655200</v>
+      </c>
+      <c r="Q4" s="4">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+      <c r="R4" s="4">
+        <f t="shared" si="2"/>
+        <v>10.4</v>
+      </c>
+      <c r="S4" s="5">
+        <v>40000</v>
+      </c>
+      <c r="T4" s="5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5">
+        <v>141</v>
+      </c>
+      <c r="D5" s="5">
+        <v>300</v>
+      </c>
+      <c r="E5" s="4">
+        <v>28.2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H5" s="5">
+        <v>20</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="J5" s="4">
+        <v>84.6</v>
+      </c>
+      <c r="K5" s="5">
+        <v>700</v>
+      </c>
+      <c r="L5" s="5">
+        <v>4091000</v>
+      </c>
+      <c r="M5" s="5">
+        <v>85000</v>
+      </c>
+      <c r="N5" s="5">
+        <v>12</v>
+      </c>
+      <c r="O5" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="0"/>
+        <v>3272800</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" si="1"/>
+        <v>68000</v>
+      </c>
+      <c r="R5" s="4">
+        <f t="shared" si="2"/>
+        <v>9.2000000000000011</v>
+      </c>
+      <c r="S5" s="5">
+        <v>70500</v>
+      </c>
+      <c r="T5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6.7</v>
+      </c>
+      <c r="D6" s="5">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.7</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="H6" s="5">
+        <v>20</v>
+      </c>
+      <c r="I6" s="5">
+        <v>6</v>
+      </c>
+      <c r="J6" s="5">
+        <v>24</v>
+      </c>
+      <c r="K6" s="5">
+        <v>630</v>
+      </c>
+      <c r="L6" s="5">
+        <v>10902000</v>
+      </c>
+      <c r="M6" s="5">
+        <v>264000</v>
+      </c>
+      <c r="N6" s="5">
+        <v>12</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="0"/>
+        <v>8721600</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="1"/>
+        <v>211200</v>
+      </c>
+      <c r="R6" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S6" s="5">
+        <v>3350</v>
+      </c>
+      <c r="T6" s="5">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>